<commit_message>
major updates to SoA.
</commit_message>
<xml_diff>
--- a/chapter-reswk/tables/tables.xlsx
+++ b/chapter-reswk/tables/tables.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\phd-thesis\chapter-reswk\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208B6CBF-9CE3-4766-B363-1EAA6E361CEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39586D16-FCA9-47EC-A01E-5DA4ED34A8F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="reqs" sheetId="1" r:id="rId1"/>
     <sheet name="Excel2LaTeX" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="mapping" sheetId="2" r:id="rId3"/>
     <sheet name="FromKarl2019" sheetId="4" r:id="rId4"/>
+    <sheet name="ETSI and ISA" sheetId="5" r:id="rId5"/>
+    <sheet name="Industry" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="OLE_LINK1" localSheetId="3">FromKarl2019!$A$1</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="278">
   <si>
     <t>Monitoring</t>
   </si>
@@ -472,12 +474,839 @@
   <si>
     <t>(Pr. Loss)</t>
   </si>
+  <si>
+    <t>Monitoring &amp; Diagnostics</t>
+  </si>
+  <si>
+    <t>Discrete Manufacturing</t>
+  </si>
+  <si>
+    <t>Logistics and Warehouse</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Augmented</t>
+  </si>
+  <si>
+    <t>Reality</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Motion</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>AGV</t>
+  </si>
+  <si>
+    <t>Cranes</t>
+  </si>
+  <si>
+    <t>Latency/Cycle</t>
+  </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>&gt; 20</t>
+  </si>
+  <si>
+    <t>1 – 12</t>
+  </si>
+  <si>
+    <t>250 μs – 1 ms</t>
+  </si>
+  <si>
+    <t>&gt; 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 – 20 </t>
+  </si>
+  <si>
+    <t>15 – 20</t>
+  </si>
+  <si>
+    <t>50 – X s</t>
+  </si>
+  <si>
+    <t>(PER)</t>
+  </si>
+  <si>
+    <t>Data Rate</t>
+  </si>
+  <si>
+    <t>(bits/sec, bps)</t>
+  </si>
+  <si>
+    <t>Kbps-Mbps</t>
+  </si>
+  <si>
+    <t>Kbps</t>
+  </si>
+  <si>
+    <t>Kbps-mbps</t>
+  </si>
+  <si>
+    <t>Mbps-Gbps</t>
+  </si>
+  <si>
+    <t>Packet Size (bytes, B)</t>
+  </si>
+  <si>
+    <t>&gt; 200 B</t>
+  </si>
+  <si>
+    <t>1-50 B</t>
+  </si>
+  <si>
+    <t>20-50 B</t>
+  </si>
+  <si>
+    <t>&lt; 300 B</t>
+  </si>
+  <si>
+    <t>&lt; 80 B</t>
+  </si>
+  <si>
+    <t>&lt; 8 B</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>&lt; 100</t>
+  </si>
+  <si>
+    <t>100 m – 1 km</t>
+  </si>
+  <si>
+    <t>&lt; 50</t>
+  </si>
+  <si>
+    <t>&lt; 200</t>
+  </si>
+  <si>
+    <t>~2</t>
+  </si>
+  <si>
+    <t>100 m -1 km</t>
+  </si>
+  <si>
+    <t>&lt; 10</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Mobility (m/s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 10 </t>
+  </si>
+  <si>
+    <t>&lt; 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 5 </t>
+  </si>
+  <si>
+    <t>&lt; 3</t>
+  </si>
+  <si>
+    <t>Density (m^-2)</t>
+  </si>
+  <si>
+    <t>0.33 – 3</t>
+  </si>
+  <si>
+    <t>10 – 20</t>
+  </si>
+  <si>
+    <t>0.33-3</t>
+  </si>
+  <si>
+    <t>&lt; 5</t>
+  </si>
+  <si>
+    <t>~ 0.1</t>
+  </si>
+  <si>
+    <t>10000/ Factory</t>
+  </si>
+  <si>
+    <t>&gt; 0.33 – 0.02</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>10 years</t>
+  </si>
+  <si>
+    <t>&lt; 8 hours</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>Use Case Class</t>
+  </si>
+  <si>
+    <t>BLER</t>
+  </si>
+  <si>
+    <t>Class 0</t>
+  </si>
+  <si>
+    <t>Class 1</t>
+  </si>
+  <si>
+    <t>Class 2 and 3</t>
+  </si>
+  <si>
+    <t>Class 4 and 5</t>
+  </si>
+  <si>
+    <t>100 avg.</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10-4</t>
+  </si>
+  <si>
+    <t>10-5</t>
+  </si>
+  <si>
+    <t>10-9</t>
+  </si>
+  <si>
+    <t>&gt;10-2</t>
+  </si>
+  <si>
+    <t>&gt;10-6</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Condition Monitoring</t>
+  </si>
+  <si>
+    <t>KPI</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Usage Class</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Factory Automation Use Cases</t>
+  </si>
+  <si>
+    <t>Class 0:  Emergency action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Always critical </t>
+  </si>
+  <si>
+    <t>Class 1:  Closed loop regulatory control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Often critical </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clause 5.3 </t>
+  </si>
+  <si>
+    <t>Class 2:  Closed loop supervisory control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usually non-critical </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clause 5.4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clause 5.5 </t>
+  </si>
+  <si>
+    <t>Class 3:  Open loop control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human in the loop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitoring </t>
+  </si>
+  <si>
+    <t>Class 4:  Alerting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short-term operational </t>
+  </si>
+  <si>
+    <t xml:space="preserve">consequence (e.g., event-based </t>
+  </si>
+  <si>
+    <t xml:space="preserve">maintenance) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clause 5.6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clause 5.7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clause 5.8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clause 5.9 </t>
+  </si>
+  <si>
+    <t>Class 5:  Logging, Downloading, and Uploading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No immediate operational </t>
+  </si>
+  <si>
+    <t xml:space="preserve">consequence (e.g., history </t>
+  </si>
+  <si>
+    <t xml:space="preserve">collection, sequence of events, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">preventive maintenance) </t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>Jitter (%)</t>
+  </si>
+  <si>
+    <t>$10^{-9}$</t>
+  </si>
+  <si>
+    <t>$+/-10$</t>
+  </si>
+  <si>
+    <t>$&lt;10$</t>
+  </si>
+  <si>
+    <t>10 to 100</t>
+  </si>
+  <si>
+    <t>$10^{-7}$</t>
+  </si>
+  <si>
+    <t>$10^{-6}$</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t># of nodes</t>
+  </si>
+  <si>
+    <t>Update rate</t>
+  </si>
+  <si>
+    <t>Goodput</t>
+  </si>
+  <si>
+    <t>System range</t>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">-1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Hz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bps</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> m</t>
+    </r>
+  </si>
+  <si>
+    <t>Process Automation</t>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Hz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bps</t>
+    </r>
+  </si>
+  <si>
+    <t>Factory Automation</t>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Hz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bps</t>
+    </r>
+  </si>
+  <si>
+    <t>Power Systems Automation</t>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Hz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> m</t>
+    </r>
+  </si>
+  <si>
+    <t>Power Electronics Control</t>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Hz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bps</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +1335,26 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -515,7 +1364,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -692,11 +1541,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -834,41 +1779,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3831,7 +4866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A42C75-BD86-4750-96C6-77A33BB6B356}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
@@ -3843,293 +4878,293 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="53" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="81" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="81" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="81" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="81" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="81" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="83" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="56">
+      <c r="C2" s="83">
         <v>4</v>
       </c>
-      <c r="D2" s="56">
+      <c r="D2" s="83">
         <v>4</v>
       </c>
-      <c r="E2" s="56">
+      <c r="E2" s="83">
         <v>20</v>
       </c>
-      <c r="F2" s="56">
+      <c r="F2" s="83">
         <v>4</v>
       </c>
-      <c r="G2" s="56">
+      <c r="G2" s="83">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="55" t="s">
+      <c r="A3" s="84"/>
+      <c r="B3" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="56">
+      <c r="C3" s="83">
         <v>0.5</v>
       </c>
-      <c r="D3" s="56">
+      <c r="D3" s="83">
         <v>0.25</v>
       </c>
-      <c r="E3" s="56">
+      <c r="E3" s="83">
         <v>4</v>
       </c>
-      <c r="F3" s="56">
+      <c r="F3" s="83">
         <v>0.5</v>
       </c>
-      <c r="G3" s="56">
+      <c r="G3" s="83">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="85" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="86" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="62">
-        <v>-7</v>
-      </c>
-      <c r="D4" s="62">
-        <v>-7</v>
-      </c>
-      <c r="E4" s="62">
-        <v>-7</v>
-      </c>
-      <c r="F4" s="62">
-        <v>-7</v>
-      </c>
-      <c r="G4" s="62">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="C4" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="G4" s="87" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="88" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="62">
-        <v>-7</v>
-      </c>
-      <c r="D5" s="62">
-        <v>-7</v>
-      </c>
-      <c r="E5" s="62">
-        <v>-7</v>
-      </c>
-      <c r="F5" s="62">
-        <v>-7</v>
-      </c>
-      <c r="G5" s="62">
-        <v>-7</v>
+      <c r="C5" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="F5" s="87" t="s">
+        <v>254</v>
+      </c>
+      <c r="G5" s="87" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="86" t="s">
         <v>126</v>
       </c>
-      <c r="C6" s="56">
+      <c r="C6" s="83">
         <v>8</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="83">
         <v>10</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="83">
         <v>10</v>
       </c>
-      <c r="F6" s="56">
+      <c r="F6" s="83">
         <v>1</v>
       </c>
-      <c r="G6" s="56">
+      <c r="G6" s="83">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="89" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="83" t="s">
         <v>131</v>
       </c>
-      <c r="C7" s="56">
+      <c r="C7" s="83">
         <v>16</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="83">
         <v>30</v>
       </c>
-      <c r="E7" s="56">
+      <c r="E7" s="83">
         <v>30</v>
       </c>
-      <c r="F7" s="56">
+      <c r="F7" s="83">
         <v>4</v>
       </c>
-      <c r="G7" s="56">
+      <c r="G7" s="83">
         <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="83" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="56">
+      <c r="C8" s="83">
         <v>10</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="83">
         <v>10</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="83">
         <v>10</v>
       </c>
-      <c r="F8" s="56">
+      <c r="F8" s="83">
         <v>10</v>
       </c>
-      <c r="G8" s="56">
+      <c r="G8" s="83">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
-      <c r="B9" s="55" t="s">
+      <c r="A9" s="82"/>
+      <c r="B9" s="83" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="56">
+      <c r="C9" s="83">
         <v>30</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="83">
         <v>30</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="83">
         <v>30</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="83">
         <v>30</v>
       </c>
-      <c r="G9" s="56">
+      <c r="G9" s="83">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="82" t="s">
         <v>133</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="56">
+      <c r="C10" s="83">
         <v>6</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="83">
         <v>8</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="83">
         <v>8</v>
       </c>
-      <c r="F10" s="56">
+      <c r="F10" s="83">
         <v>8</v>
       </c>
-      <c r="G10" s="56">
+      <c r="G10" s="83">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="55" t="s">
+      <c r="A11" s="84"/>
+      <c r="B11" s="83" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="56">
+      <c r="C11" s="83">
         <v>24</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="83">
         <v>1024</v>
       </c>
-      <c r="E11" s="56">
+      <c r="E11" s="83">
         <v>1024</v>
       </c>
-      <c r="F11" s="56">
+      <c r="F11" s="83">
         <v>1024</v>
       </c>
-      <c r="G11" s="56">
+      <c r="G11" s="83">
         <v>33000</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="86" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="56">
+      <c r="C12" s="83">
         <v>125</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="83">
         <v>125</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="83">
         <v>25</v>
       </c>
-      <c r="F12" s="56">
+      <c r="F12" s="83">
         <v>125</v>
       </c>
-      <c r="G12" s="56">
+      <c r="G12" s="83">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="83" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="56">
+      <c r="C13" s="83">
         <v>1000</v>
       </c>
-      <c r="D13" s="56">
+      <c r="D13" s="83">
         <v>2000</v>
       </c>
-      <c r="E13" s="56">
+      <c r="E13" s="83">
         <v>125</v>
       </c>
-      <c r="F13" s="56">
+      <c r="F13" s="83">
         <v>1000</v>
       </c>
-      <c r="G13" s="56">
+      <c r="G13" s="83">
         <v>125</v>
       </c>
     </row>
@@ -4143,4 +5178,876 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A638E0-57CA-4B74-909A-151DE85BE9D3}">
+  <dimension ref="A1:V25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="4" customWidth="1"/>
+    <col min="2" max="11" width="10.28515625" style="3" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="3"/>
+    <col min="14" max="14" width="13.42578125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="3" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="3"/>
+    <col min="19" max="19" width="21.85546875" style="3" customWidth="1"/>
+    <col min="20" max="22" width="12.42578125" style="3" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="63"/>
+      <c r="B1" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="64" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="O1" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="P1" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q1" s="70" t="s">
+        <v>222</v>
+      </c>
+      <c r="S1" s="78" t="s">
+        <v>202</v>
+      </c>
+      <c r="T1" s="79" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="79" t="s">
+        <v>249</v>
+      </c>
+      <c r="V1" s="78" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="63" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="64" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="K2" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="71" t="s">
+        <v>223</v>
+      </c>
+      <c r="P2" s="71" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q2" s="71"/>
+      <c r="S2" s="62" t="s">
+        <v>204</v>
+      </c>
+      <c r="T2" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="U2" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="V2" s="76" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="68" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3" s="68" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="J3" s="68" t="s">
+        <v>210</v>
+      </c>
+      <c r="K3" s="68" t="s">
+        <v>210</v>
+      </c>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="72"/>
+      <c r="S3" s="62" t="s">
+        <v>205</v>
+      </c>
+      <c r="T3" s="80">
+        <v>10</v>
+      </c>
+      <c r="U3" s="80" t="s">
+        <v>251</v>
+      </c>
+      <c r="V3" s="80" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="N4" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="O4" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="P4" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q4" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="S4" s="62" t="s">
+        <v>206</v>
+      </c>
+      <c r="T4" s="80" t="s">
+        <v>253</v>
+      </c>
+      <c r="U4" s="80" t="s">
+        <v>252</v>
+      </c>
+      <c r="V4" s="80" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="68" t="s">
+        <v>214</v>
+      </c>
+      <c r="G5" s="68" t="s">
+        <v>215</v>
+      </c>
+      <c r="H5" s="68" t="s">
+        <v>215</v>
+      </c>
+      <c r="I5" s="68" t="s">
+        <v>212</v>
+      </c>
+      <c r="J5" s="68" t="s">
+        <v>212</v>
+      </c>
+      <c r="K5" s="68" t="s">
+        <v>213</v>
+      </c>
+      <c r="N5" s="73"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
+      <c r="S5" s="62" t="s">
+        <v>207</v>
+      </c>
+      <c r="T5" s="80" t="s">
+        <v>208</v>
+      </c>
+      <c r="U5" s="80" t="s">
+        <v>251</v>
+      </c>
+      <c r="V5" s="80" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="67" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="71" t="s">
+        <v>228</v>
+      </c>
+      <c r="P6" s="71" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q6" s="75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="J7" s="68" t="s">
+        <v>166</v>
+      </c>
+      <c r="K7" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="75" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="67" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="72"/>
+      <c r="Q8" s="76"/>
+    </row>
+    <row r="9" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="67" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="68" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="G9" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="H9" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="I9" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J9" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="K9" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="N9" s="73"/>
+      <c r="O9" s="71" t="s">
+        <v>232</v>
+      </c>
+      <c r="P9" s="71" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q9" s="75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="67" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="68" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10" s="68" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" s="68" t="s">
+        <v>180</v>
+      </c>
+      <c r="J10" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="K10" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="75" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="68"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="72"/>
+      <c r="Q11" s="76"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="67" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" s="68" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>184</v>
+      </c>
+      <c r="E12" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="H12" s="68" t="s">
+        <v>186</v>
+      </c>
+      <c r="I12" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="J12" s="68" t="s">
+        <v>187</v>
+      </c>
+      <c r="K12" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="N12" s="71" t="s">
+        <v>234</v>
+      </c>
+      <c r="O12" s="71" t="s">
+        <v>235</v>
+      </c>
+      <c r="P12" s="75" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q12" s="75" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="75" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q13" s="75" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="67" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" s="68" t="s">
+        <v>192</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="G14" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="H14" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="I14" s="68" t="s">
+        <v>194</v>
+      </c>
+      <c r="J14" s="68" t="s">
+        <v>195</v>
+      </c>
+      <c r="K14" s="68" t="s">
+        <v>195</v>
+      </c>
+      <c r="N14" s="73"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="75" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q14" s="75" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15" s="68"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
+      <c r="N15" s="73"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="75"/>
+      <c r="Q15" s="75" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="67" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" s="68" t="s">
+        <v>198</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>199</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>198</v>
+      </c>
+      <c r="E16" s="68" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" s="68" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" s="68" t="s">
+        <v>200</v>
+      </c>
+      <c r="H16" s="68" t="s">
+        <v>198</v>
+      </c>
+      <c r="I16" s="68" t="s">
+        <v>199</v>
+      </c>
+      <c r="J16" s="68" t="s">
+        <v>201</v>
+      </c>
+      <c r="K16" s="68" t="s">
+        <v>198</v>
+      </c>
+      <c r="N16" s="73"/>
+      <c r="O16" s="72"/>
+      <c r="P16" s="77"/>
+      <c r="Q16" s="76"/>
+    </row>
+    <row r="17" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="65" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="71" t="s">
+        <v>243</v>
+      </c>
+      <c r="P17" s="75" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q17" s="75" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="75" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q18" s="75" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="73"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="75" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q19" s="75" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="60"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="57"/>
+      <c r="N20" s="72"/>
+      <c r="O20" s="72"/>
+      <c r="P20" s="76" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q20" s="76" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="61"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="58"/>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="62"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="62"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="62"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="62"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="P9:P11"/>
+    <mergeCell ref="N12:N20"/>
+    <mergeCell ref="O12:O16"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="N4:N11"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="P6:P8"/>
+    <mergeCell ref="O9:O11"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5609B911-E5E7-4C19-BBA8-0DEC78E06F5B}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="94" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="94"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="90" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="91" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" s="91" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="92" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="93" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="93" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="93" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="93" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="92" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="93" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" s="93" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="93" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="93" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="92" t="s">
+        <v>268</v>
+      </c>
+      <c r="B4" s="93" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" s="93" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" s="93" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="92" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" s="93" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" s="93" t="s">
+        <v>273</v>
+      </c>
+      <c r="D5" s="93" t="s">
+        <v>270</v>
+      </c>
+      <c r="E5" s="93" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="92" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" s="93" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6" s="93" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" s="93" t="s">
+        <v>277</v>
+      </c>
+      <c r="E6" s="93" t="s">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>